<commit_message>
Final code for deriving SoA and RTs from the data!
</commit_message>
<xml_diff>
--- a/SoA_EEG.xlsx
+++ b/SoA_EEG.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>comp_l</t>
   </si>
@@ -32,6 +32,33 @@
   </si>
   <si>
     <t>neut_r</t>
+  </si>
+  <si>
+    <t>comp_r_RT</t>
+  </si>
+  <si>
+    <t>comp_l_RT</t>
+  </si>
+  <si>
+    <t>incomp_r_RT</t>
+  </si>
+  <si>
+    <t>incomp_l_RT</t>
+  </si>
+  <si>
+    <t>neut_r_RT</t>
+  </si>
+  <si>
+    <t>neut_l_RT</t>
+  </si>
+  <si>
+    <t>comp_RT</t>
+  </si>
+  <si>
+    <t>incomp_RT</t>
+  </si>
+  <si>
+    <t>neut_RT</t>
   </si>
   <si>
     <t>comp</t>
@@ -512,13 +539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:BD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:56">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,8 +684,35 @@
       <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="AV1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:56">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -681,123 +735,150 @@
         <v>67.5</v>
       </c>
       <c r="H2">
+        <v>319.426666666667</v>
+      </c>
+      <c r="I2">
+        <v>326.554054054054</v>
+      </c>
+      <c r="J2">
+        <v>352.848484848485</v>
+      </c>
+      <c r="K2">
+        <v>341.161764705882</v>
+      </c>
+      <c r="L2">
+        <v>351.088235294118</v>
+      </c>
+      <c r="M2">
+        <v>337.376811594203</v>
+      </c>
+      <c r="N2">
+        <v>322.99036036036</v>
+      </c>
+      <c r="O2">
+        <v>347.005124777184</v>
+      </c>
+      <c r="P2">
+        <v>344.23252344416</v>
+      </c>
+      <c r="Q2">
         <v>57.8333333333333</v>
       </c>
-      <c r="I2">
+      <c r="R2">
         <v>53.3333333333333</v>
       </c>
-      <c r="J2">
+      <c r="S2">
         <v>58.3333333333333</v>
       </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2">
+      <c r="T2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2">
         <v>90</v>
       </c>
-      <c r="M2">
+      <c r="V2">
         <v>35</v>
       </c>
-      <c r="N2">
+      <c r="W2">
         <v>30</v>
       </c>
-      <c r="O2">
+      <c r="X2">
         <v>95</v>
       </c>
-      <c r="P2">
+      <c r="Y2">
         <v>79</v>
       </c>
-      <c r="Q2">
+      <c r="Z2">
         <v>30</v>
       </c>
-      <c r="R2">
+      <c r="AA2">
         <v>10</v>
       </c>
-      <c r="S2">
+      <c r="AB2">
         <v>85</v>
-      </c>
-      <c r="T2">
-        <v>60</v>
-      </c>
-      <c r="U2">
-        <v>20</v>
-      </c>
-      <c r="V2">
-        <v>70</v>
-      </c>
-      <c r="W2">
-        <v>90</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>70</v>
-      </c>
-      <c r="Z2">
-        <v>80</v>
-      </c>
-      <c r="AA2">
-        <v>25</v>
-      </c>
-      <c r="AB2">
-        <v>65</v>
       </c>
       <c r="AC2">
         <v>60</v>
       </c>
       <c r="AD2">
+        <v>20</v>
+      </c>
+      <c r="AE2">
+        <v>70</v>
+      </c>
+      <c r="AF2">
+        <v>90</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>70</v>
+      </c>
+      <c r="AI2">
         <v>80</v>
       </c>
-      <c r="AE2">
+      <c r="AJ2">
+        <v>25</v>
+      </c>
+      <c r="AK2">
         <v>65</v>
       </c>
-      <c r="AF2">
-        <v>10</v>
-      </c>
-      <c r="AG2">
+      <c r="AL2">
         <v>60</v>
-      </c>
-      <c r="AH2">
-        <v>50</v>
-      </c>
-      <c r="AI2">
-        <v>75</v>
-      </c>
-      <c r="AJ2">
-        <v>60</v>
-      </c>
-      <c r="AK2">
-        <v>5</v>
-      </c>
-      <c r="AL2">
-        <v>100</v>
       </c>
       <c r="AM2">
         <v>80</v>
       </c>
       <c r="AN2">
+        <v>65</v>
+      </c>
+      <c r="AO2">
         <v>10</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
+        <v>60</v>
+      </c>
+      <c r="AQ2">
+        <v>50</v>
+      </c>
+      <c r="AR2">
+        <v>75</v>
+      </c>
+      <c r="AS2">
+        <v>60</v>
+      </c>
+      <c r="AT2">
+        <v>5</v>
+      </c>
+      <c r="AU2">
+        <v>100</v>
+      </c>
+      <c r="AV2">
+        <v>80</v>
+      </c>
+      <c r="AW2">
+        <v>10</v>
+      </c>
+      <c r="AX2">
         <v>40</v>
       </c>
-      <c r="AP2">
+      <c r="AY2">
         <v>85</v>
       </c>
-      <c r="AQ2">
+      <c r="AZ2">
         <v>40</v>
       </c>
-      <c r="AR2">
+      <c r="BA2">
         <v>40</v>
       </c>
-      <c r="AS2">
+      <c r="BB2">
         <v>40</v>
       </c>
-      <c r="AT2">
+      <c r="BC2">
         <v>100</v>
       </c>
-      <c r="AU2">
+      <c r="BD2">
         <v>100</v>
       </c>
     </row>

</xml_diff>